<commit_message>
Revert "PRUEBAS AL 08/07/2016"
This reverts commit e3566331f504e25aedc19a16fe97b6c2b7e016cc.
</commit_message>
<xml_diff>
--- a/FASE_2_SPRINT_3/PRUEBAS_TECNICAS/Comprobación_Cálculos.xlsx
+++ b/FASE_2_SPRINT_3/PRUEBAS_TECNICAS/Comprobación_Cálculos.xlsx
@@ -1,28 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SIGANEM\GITHUB\SIGANEM\FASE_2_SPRINT_3\PRUEBAS_TECNICAS\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="45" windowWidth="23715" windowHeight="10035" activeTab="2"/>
+    <workbookView xWindow="120" yWindow="45" windowWidth="23715" windowHeight="10035"/>
   </bookViews>
   <sheets>
-    <sheet name="Valor_Nominal_Reales" sheetId="1" r:id="rId1"/>
-    <sheet name="Valor_Nominal_Valor" sheetId="2" r:id="rId2"/>
-    <sheet name="Valor_Nominal_Fideicomiso" sheetId="4" r:id="rId3"/>
-    <sheet name="Hoja3" sheetId="3" r:id="rId4"/>
+    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
+    <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>% Aceptación BCR</t>
   </si>
@@ -37,42 +31,6 @@
   </si>
   <si>
     <t>Saldo Colonizado</t>
-  </si>
-  <si>
-    <t>Monto Ultima Tasación Terreno</t>
-  </si>
-  <si>
-    <t>Monto Ultima Tasación No Terreno</t>
-  </si>
-  <si>
-    <t>Valor Nominal</t>
-  </si>
-  <si>
-    <t>(A2*(B2+C2) / 100)</t>
-  </si>
-  <si>
-    <t>Valor Mercado Colonizado</t>
-  </si>
-  <si>
-    <t>Valor Nominal Garantía</t>
-  </si>
-  <si>
-    <t>((A2*B2) / 100)</t>
-  </si>
-  <si>
-    <t>ID GARANTIA</t>
-  </si>
-  <si>
-    <t>VALOR NOMINAL</t>
-  </si>
-  <si>
-    <t>VALOR NOMINAL FIDEICOMISO =</t>
-  </si>
-  <si>
-    <t>000400</t>
-  </si>
-  <si>
-    <t>5200</t>
   </si>
 </sst>
 </file>
@@ -120,7 +78,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -151,24 +109,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.249977111117893"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -190,7 +130,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="3"/>
@@ -198,22 +138,14 @@
     <xf numFmtId="43" fontId="4" fillId="5" borderId="0" xfId="5" applyNumberFormat="1"/>
     <xf numFmtId="43" fontId="1" fillId="3" borderId="0" xfId="4" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="4" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="43" fontId="4" fillId="7" borderId="0" xfId="5" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="3" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="3" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="40% - Accent1" xfId="4" builtinId="31"/>
-    <cellStyle name="Accent6" xfId="5" builtinId="49"/>
-    <cellStyle name="Comma" xfId="1" builtinId="3"/>
-    <cellStyle name="Good" xfId="3" builtinId="26"/>
+    <cellStyle name="40% - Énfasis1" xfId="4" builtinId="31"/>
+    <cellStyle name="Buena" xfId="3" builtinId="26"/>
+    <cellStyle name="Énfasis6" xfId="5" builtinId="49"/>
+    <cellStyle name="Millares" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Percent" xfId="2" builtinId="5"/>
+    <cellStyle name="Porcentaje" xfId="2" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -221,15 +153,12 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -271,7 +200,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -306,7 +235,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -515,104 +444,40 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="32.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="6">
-        <v>10</v>
-      </c>
-      <c r="B2" s="7">
-        <v>0</v>
-      </c>
-      <c r="C2" s="4">
-        <v>22500000</v>
-      </c>
-      <c r="D2" s="5">
-        <f>(A2*(B2+C2) / 100)</f>
-        <v>2250000</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F3" s="1"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D5" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D6" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="39" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>9</v>
-      </c>
       <c r="C1" s="3" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="6">
-        <v>80</v>
-      </c>
-      <c r="B2" s="7">
-        <v>135347.5</v>
+      <c r="A2" s="4">
+        <v>1165251.97</v>
+      </c>
+      <c r="B2" s="6">
+        <v>75</v>
       </c>
       <c r="C2" s="5">
-        <f>((A2*B2) / 100)</f>
-        <v>108278</v>
+        <f>(A2*B2)/100</f>
+        <v>873938.97750000004</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -625,138 +490,35 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C6" s="2" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="39" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O29" sqref="O29"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="29.7109375" customWidth="1"/>
-    <col min="2" max="2" width="16.28515625" style="12" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="B1" s="11" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2" s="13">
-        <v>1146000</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="B3" s="13">
-        <v>27069500</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="9"/>
-      <c r="B4" s="13"/>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="9"/>
-      <c r="B5" s="13"/>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="9"/>
-      <c r="B6" s="13"/>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="9"/>
-      <c r="B7" s="13"/>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="9"/>
-      <c r="B8" s="13"/>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="9"/>
-      <c r="B9" s="13"/>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B10" s="14">
-        <f>SUM(B2:B9)</f>
-        <v>28215500</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="4">
-        <v>1165251.97</v>
-      </c>
-      <c r="B2" s="6">
-        <v>75</v>
-      </c>
-      <c r="C2" s="5">
-        <f>(A2*B2)/100</f>
-        <v>873938.97750000004</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E3" s="1"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C5" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C6" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>